<commit_message>
TypeCheck.hs, T/L, journal updates
Still working on typeCheck. Updated journal, added question.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-30may2016 .xlsx
+++ b/time-labor/week-of-30may2016 .xlsx
@@ -21,6 +21,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -590,17 +591,17 @@
   <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -845,13 +846,17 @@
       <c r="B15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
+      <c r="C15" s="19" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D15" s="20" t="n">
+        <v>0.791666666666667</v>
+      </c>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="21" t="n">
         <f aca="false">IF((((D15-C15)+(F15-E15))*24)&gt;8,8,((D15-C15)+(F15-E15))*24)</f>
-        <v>0</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="H15" s="21" t="n">
         <f aca="false">IF(((D15-C15)+(F15-E15))*24&gt;8,((D15-C15)+(F15-E15))*24-8,0)</f>
@@ -885,13 +890,17 @@
       <c r="B17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="19" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D17" s="20" t="n">
+        <v>0.791666666666667</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21" t="n">
         <f aca="false">IF((((D17-C17)+(F17-E17))*24)&gt;8,8,((D17-C17)+(F17-E17))*24)</f>
-        <v>0</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="H17" s="21" t="n">
         <f aca="false">IF(((D17-C17)+(F17-E17))*24&gt;8,((D17-C17)+(F17-E17))*24-8,0)</f>
@@ -905,13 +914,17 @@
       <c r="B18" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="19" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="D18" s="20" t="n">
+        <v>0.5</v>
+      </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
       <c r="G18" s="21" t="n">
         <f aca="false">IF((((D18-C18)+(F18-E18))*24)&gt;8,8,((D18-C18)+(F18-E18))*24)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="21" t="n">
         <f aca="false">IF(((D18-C18)+(F18-E18))*24&gt;8,((D18-C18)+(F18-E18))*24-8,0)</f>
@@ -926,16 +939,16 @@
         <v>29</v>
       </c>
       <c r="C19" s="19" t="n">
-        <v>0</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="D19" s="20" t="n">
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21" t="n">
         <f aca="false">IF((((D19-C19)+(F19-E19))*24)&gt;8,8,((D19-C19)+(F19-E19))*24)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H19" s="21" t="n">
         <f aca="false">IF(((D19-C19)+(F19-E19))*24&gt;8,((D19-C19)+(F19-E19))*24-8,0)</f>
@@ -955,7 +968,7 @@
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>6.5</v>
+        <v>16.5</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -999,7 +1012,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>65</v>
+        <v>165</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1015,7 +1028,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>65</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>